<commit_message>
Updates to phone number check
</commit_message>
<xml_diff>
--- a/app/config/tables/MASKINCL/Forms/MASKINCL/MASKINCL.xlsx
+++ b/app/config/tables/MASKINCL/Forms/MASKINCL/MASKINCL.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7A94C7-39D6-4ADB-A0A1-02C12FE321F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFAE7901-07B0-4C20-B165-28356A346571}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="190">
   <si>
     <t>setting_name</t>
   </si>
@@ -562,6 +562,48 @@
   </si>
   <si>
     <t>display.hide_adate</t>
+  </si>
+  <si>
+    <t>YesNo</t>
+  </si>
+  <si>
+    <t>newNumber</t>
+  </si>
+  <si>
+    <t>Add other number?</t>
+  </si>
+  <si>
+    <t>Número de telefone</t>
+  </si>
+  <si>
+    <t>Adicionar outro número?</t>
+  </si>
+  <si>
+    <t>data("newNumber") == "1"</t>
+  </si>
+  <si>
+    <t>TELE1_VERI</t>
+  </si>
+  <si>
+    <t>TELE2_VERI</t>
+  </si>
+  <si>
+    <t>NOVONUM1</t>
+  </si>
+  <si>
+    <t>NOVONUM2</t>
+  </si>
+  <si>
+    <t>New number 1</t>
+  </si>
+  <si>
+    <t>New number 2</t>
+  </si>
+  <si>
+    <t>Novo número 1</t>
+  </si>
+  <si>
+    <t>Novo número 2</t>
   </si>
 </sst>
 </file>
@@ -1106,11 +1148,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
-  <dimension ref="A1:N50"/>
+  <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M34" sqref="M34"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F26" sqref="F26:F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1120,7 +1162,7 @@
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="46.28515625" customWidth="1"/>
     <col min="8" max="8" width="41" customWidth="1"/>
     <col min="9" max="9" width="29.85546875" customWidth="1"/>
@@ -1128,6 +1170,7 @@
     <col min="11" max="11" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1393,7 +1436,7 @@
         <v>77</v>
       </c>
       <c r="H25" t="s">
-        <v>77</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -1404,7 +1447,7 @@
         <v>78</v>
       </c>
       <c r="F26" t="s">
-        <v>79</v>
+        <v>182</v>
       </c>
       <c r="G26" t="s">
         <v>79</v>
@@ -1421,7 +1464,7 @@
         <v>78</v>
       </c>
       <c r="F27" t="s">
-        <v>81</v>
+        <v>183</v>
       </c>
       <c r="G27" t="s">
         <v>81</v>
@@ -1431,213 +1474,281 @@
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>39</v>
+      <c r="D28" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" t="s">
+        <v>176</v>
+      </c>
+      <c r="F28" t="s">
+        <v>177</v>
+      </c>
+      <c r="G28" t="s">
+        <v>178</v>
+      </c>
+      <c r="H28" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D30" t="s">
-        <v>53</v>
-      </c>
-      <c r="E30" t="s">
-        <v>82</v>
-      </c>
-      <c r="F30" t="s">
-        <v>83</v>
-      </c>
-      <c r="G30" t="s">
-        <v>84</v>
-      </c>
-      <c r="H30" t="s">
-        <v>85</v>
+      <c r="B30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>57</v>
-      </c>
-      <c r="C31" t="s">
-        <v>141</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>53</v>
-      </c>
-      <c r="E32" t="s">
-        <v>164</v>
+        <v>142</v>
       </c>
       <c r="F32" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="G32" t="s">
-        <v>87</v>
+        <v>186</v>
       </c>
       <c r="H32" t="s">
-        <v>86</v>
+        <v>188</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>58</v>
+      <c r="D33" t="s">
+        <v>142</v>
+      </c>
+      <c r="F33" t="s">
+        <v>185</v>
+      </c>
+      <c r="G33" t="s">
+        <v>187</v>
+      </c>
+      <c r="H33" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D35" t="s">
-        <v>91</v>
-      </c>
-      <c r="F35" t="s">
-        <v>83</v>
-      </c>
-      <c r="I35">
-        <v>2</v>
+      <c r="B35" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+      <c r="D37" t="s">
+        <v>53</v>
+      </c>
+      <c r="E37" t="s">
+        <v>82</v>
+      </c>
+      <c r="F37" t="s">
+        <v>83</v>
+      </c>
+      <c r="G37" t="s">
+        <v>84</v>
+      </c>
+      <c r="H37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>57</v>
       </c>
-      <c r="C37" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D38" t="s">
-        <v>91</v>
-      </c>
-      <c r="F38" t="s">
-        <v>83</v>
-      </c>
-      <c r="I38">
-        <v>8</v>
+      <c r="C38" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>58</v>
+      <c r="D39" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" t="s">
+        <v>164</v>
+      </c>
+      <c r="F39" t="s">
+        <v>173</v>
+      </c>
+      <c r="G39" t="s">
+        <v>87</v>
+      </c>
+      <c r="H39" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>38</v>
+        <v>57</v>
+      </c>
+      <c r="C41" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>53</v>
-      </c>
-      <c r="E42" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F42" t="s">
-        <v>95</v>
-      </c>
-      <c r="G42" t="s">
-        <v>97</v>
-      </c>
-      <c r="H42" t="s">
-        <v>96</v>
+        <v>83</v>
+      </c>
+      <c r="I42">
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
         <v>57</v>
       </c>
-      <c r="C43" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D44" t="s">
-        <v>53</v>
-      </c>
-      <c r="E44" t="s">
-        <v>108</v>
-      </c>
-      <c r="F44" t="s">
-        <v>103</v>
-      </c>
-      <c r="G44" t="s">
-        <v>64</v>
-      </c>
-      <c r="H44" t="s">
-        <v>66</v>
+      <c r="C44" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>58</v>
+      <c r="D45" t="s">
+        <v>91</v>
+      </c>
+      <c r="F45" t="s">
+        <v>83</v>
+      </c>
+      <c r="I45">
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>57</v>
-      </c>
-      <c r="C46" t="s">
-        <v>104</v>
+        <v>58</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D47" t="s">
-        <v>53</v>
-      </c>
-      <c r="E47" t="s">
-        <v>109</v>
-      </c>
-      <c r="F47" t="s">
-        <v>105</v>
-      </c>
-      <c r="G47" t="s">
-        <v>106</v>
-      </c>
-      <c r="H47" t="s">
-        <v>107</v>
+      <c r="B47" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="49" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
-        <v>170</v>
+        <v>53</v>
       </c>
       <c r="E49" t="s">
-        <v>171</v>
+        <v>93</v>
       </c>
       <c r="F49" t="s">
-        <v>94</v>
-      </c>
-      <c r="N49" s="19" t="b">
-        <v>1</v>
+        <v>95</v>
+      </c>
+      <c r="G49" t="s">
+        <v>97</v>
+      </c>
+      <c r="H49" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>53</v>
+      </c>
+      <c r="E51" t="s">
+        <v>108</v>
+      </c>
+      <c r="F51" t="s">
+        <v>103</v>
+      </c>
+      <c r="G51" t="s">
+        <v>64</v>
+      </c>
+      <c r="H51" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>57</v>
+      </c>
+      <c r="C53" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>53</v>
+      </c>
+      <c r="E54" t="s">
+        <v>109</v>
+      </c>
+      <c r="F54" t="s">
+        <v>105</v>
+      </c>
+      <c r="G54" t="s">
+        <v>106</v>
+      </c>
+      <c r="H54" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>170</v>
+      </c>
+      <c r="E56" t="s">
+        <v>171</v>
+      </c>
+      <c r="F56" t="s">
+        <v>94</v>
+      </c>
+      <c r="N56" s="19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1648,11 +1759,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D105"/>
+  <dimension ref="A1:D108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1901,12 +2012,12 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>82</v>
+        <v>176</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" t="s">
         <v>71</v>
       </c>
       <c r="D20" t="s">
@@ -1915,29 +2026,15 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>82</v>
-      </c>
-      <c r="B21">
+        <v>176</v>
+      </c>
+      <c r="B21" s="10">
         <v>2</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="D21" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>82</v>
-      </c>
-      <c r="B22">
-        <v>3</v>
-      </c>
-      <c r="C22" s="12" t="s">
+      <c r="C21" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D21" s="10" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1946,179 +2043,179 @@
         <v>82</v>
       </c>
       <c r="B23">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>101</v>
+        <v>71</v>
+      </c>
+      <c r="D23" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C24" s="16"/>
-      <c r="D24" s="14"/>
+      <c r="A24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>74</v>
+        <v>72</v>
+      </c>
+      <c r="D25" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>93</v>
-      </c>
-      <c r="B27">
-        <v>3</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>100</v>
-      </c>
+      <c r="C27" s="16"/>
+      <c r="D27" s="14"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>93</v>
       </c>
-      <c r="B28" s="7">
-        <v>8</v>
+      <c r="B28">
+        <v>1</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
+      <c r="A29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>108</v>
-      </c>
-      <c r="B30" s="13">
-        <v>1</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>112</v>
+        <v>93</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>93</v>
+      </c>
+      <c r="B31" s="7">
+        <v>8</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="7"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>108</v>
       </c>
-      <c r="B31" s="13">
-        <v>2</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>108</v>
-      </c>
-      <c r="B32" s="13">
-        <v>8</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
+      <c r="B33" s="13">
+        <v>1</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B34" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B35" s="13">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>109</v>
-      </c>
-      <c r="B36" s="13">
-        <v>3</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>120</v>
-      </c>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>109</v>
       </c>
       <c r="B37" s="13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2126,29 +2223,56 @@
         <v>109</v>
       </c>
       <c r="B38" s="13">
+        <v>2</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" s="13">
+        <v>3</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>109</v>
+      </c>
+      <c r="B40" s="13">
+        <v>4</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>109</v>
+      </c>
+      <c r="B41" s="13">
         <v>8</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C41" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="D38" s="17" t="s">
+      <c r="D41" s="17" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" s="13"/>
@@ -2206,34 +2330,38 @@
       <c r="D52" s="13"/>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="7"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="7"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="7"/>
+      <c r="B55" s="13"/>
       <c r="C55" s="13"/>
       <c r="D55" s="13"/>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" s="7"/>
-      <c r="C56" s="13"/>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" s="7"/>
-      <c r="C57" s="13"/>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="7"/>
-      <c r="C59" s="7"/>
+      <c r="C59" s="13"/>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="7"/>
+      <c r="C60" s="13"/>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" s="7"/>
@@ -2245,14 +2373,13 @@
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" s="7"/>
-      <c r="C63" s="7"/>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B65" s="15"/>
+      <c r="B65" s="7"/>
       <c r="C65" s="7"/>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
@@ -2264,7 +2391,7 @@
       <c r="C67" s="7"/>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B68" s="7"/>
+      <c r="B68" s="15"/>
       <c r="C68" s="7"/>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
@@ -2329,24 +2456,27 @@
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B84" s="7"/>
-      <c r="C84" s="15"/>
+      <c r="C84" s="7"/>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B85" s="7"/>
+      <c r="C85" s="7"/>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B86" s="7"/>
-      <c r="C86" s="15"/>
-      <c r="D86" s="15"/>
+      <c r="C86" s="7"/>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B87" s="7"/>
+      <c r="C87" s="15"/>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B88" s="7"/>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B89" s="7"/>
+      <c r="C89" s="15"/>
+      <c r="D89" s="15"/>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B90" s="7"/>
@@ -2395,6 +2525,15 @@
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" s="7"/>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B106" s="7"/>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B107" s="7"/>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B108" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -2620,11 +2759,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2784,11 +2923,19 @@
       <c r="I10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I11"/>
+      <c r="A11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>142</v>
@@ -2796,63 +2943,49 @@
       <c r="C12" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="H12"/>
-      <c r="I12"/>
+      <c r="G12"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H13"/>
+      <c r="G13"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>61</v>
+        <v>142</v>
       </c>
       <c r="C14" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="H14"/>
-      <c r="I14"/>
+      <c r="G14"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>142</v>
+        <v>30</v>
       </c>
       <c r="C15" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="H15"/>
-      <c r="I15"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>142</v>
+        <v>61</v>
       </c>
       <c r="C16" s="3" t="b">
         <v>0</v>
       </c>
       <c r="H16"/>
-      <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>142</v>
@@ -2864,11 +2997,21 @@
       <c r="I17"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>182</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C18" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18"/>
       <c r="I18"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>83</v>
+        <v>183</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>142</v>
@@ -2877,14 +3020,14 @@
         <v>0</v>
       </c>
       <c r="H19"/>
-      <c r="I19"/>
+      <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>94</v>
+        <v>184</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>61</v>
+        <v>142</v>
       </c>
       <c r="C20" s="3" t="b">
         <v>0</v>
@@ -2894,7 +3037,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>95</v>
+        <v>185</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>142</v>
@@ -2902,23 +3045,15 @@
       <c r="C21" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="H21"/>
+      <c r="I21"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>103</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C22" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H22"/>
+      <c r="B22"/>
+      <c r="I22"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>142</v>
@@ -2930,11 +3065,21 @@
       <c r="I23"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24"/>
       <c r="I24"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>151</v>
+      <c r="A25" t="s">
+        <v>95</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>142</v>
@@ -2942,49 +3087,100 @@
       <c r="C25" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I25"/>
+      <c r="H25"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C26" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H26"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C27" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H27"/>
+      <c r="I27"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I28"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C29" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I29"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B30" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="3" t="b">
+      <c r="C30" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="I26"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I29"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I30"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I31"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I32"/>
+      <c r="A31" t="s">
+        <v>177</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C31" s="3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I33"/>
     </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I34"/>
+    </row>
+    <row r="35" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I35"/>
+    </row>
+    <row r="36" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I36"/>
+    </row>
     <row r="37" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I37" s="10"/>
-    </row>
-    <row r="42" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I42"/>
-    </row>
-    <row r="43" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I43"/>
-    </row>
-    <row r="44" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I44"/>
+      <c r="I37"/>
+    </row>
+    <row r="41" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I41" s="10"/>
+    </row>
+    <row r="46" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I46"/>
+    </row>
+    <row r="47" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I47"/>
+    </row>
+    <row r="48" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I48"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I1:I44">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I1:I48">
     <sortCondition ref="I1"/>
   </sortState>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
Udates to INCL in office
</commit_message>
<xml_diff>
--- a/app/config/tables/MASKINCL/Forms/MASKINCL/MASKINCL.xlsx
+++ b/app/config/tables/MASKINCL/Forms/MASKINCL/MASKINCL.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704D539B-E148-42B0-B6A8-B3668763F08F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604E6E89-83AA-454F-8D05-2DEC57F51751}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="254">
   <si>
     <t>setting_name</t>
   </si>
@@ -766,6 +766,36 @@
   </si>
   <si>
     <t>(data("ESTADO") == "1" || data("ESTADO") == "4" || data("ESTADO") == "5"  || data("ESTADO") == "99") &amp;&amp; data("OBS_IDADE") == null</t>
+  </si>
+  <si>
+    <t>data("TELE1") != null</t>
+  </si>
+  <si>
+    <t>data("TELE2") != null</t>
+  </si>
+  <si>
+    <t>select_multiple</t>
+  </si>
+  <si>
+    <t>dontKnowDate</t>
+  </si>
+  <si>
+    <t>datasains</t>
+  </si>
+  <si>
+    <t>Don't know the date</t>
+  </si>
+  <si>
+    <t>Não sabe a data</t>
+  </si>
+  <si>
+    <t>data("datasains") != null</t>
+  </si>
+  <si>
+    <t>assign</t>
+  </si>
+  <si>
+    <t>data("datasains")</t>
   </si>
 </sst>
 </file>
@@ -1309,11 +1339,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
-  <dimension ref="A1:O62"/>
+  <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A44" sqref="A44:XFD44"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1522,7 +1552,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>46</v>
       </c>
@@ -1533,22 +1563,22 @@
         <v>199</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>53</v>
       </c>
@@ -1565,7 +1595,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>57</v>
       </c>
@@ -1573,7 +1603,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>30</v>
       </c>
@@ -1586,385 +1616,449 @@
       <c r="H23" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="M23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>246</v>
+      </c>
+      <c r="E24" t="s">
+        <v>247</v>
+      </c>
+      <c r="F24" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>57</v>
       </c>
-      <c r="C24" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
-        <v>61</v>
-      </c>
-      <c r="F25" t="s">
-        <v>63</v>
-      </c>
-      <c r="G25" t="s">
-        <v>65</v>
-      </c>
-      <c r="H25" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>252</v>
+      </c>
+      <c r="F26" t="s">
+        <v>62</v>
+      </c>
+      <c r="I26" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>61</v>
       </c>
       <c r="F29" t="s">
-        <v>193</v>
+        <v>63</v>
       </c>
       <c r="G29" t="s">
-        <v>194</v>
+        <v>65</v>
       </c>
       <c r="H29" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>57</v>
       </c>
       <c r="C32" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D34" t="s">
-        <v>53</v>
-      </c>
-      <c r="E34" t="s">
-        <v>70</v>
-      </c>
-      <c r="F34" t="s">
-        <v>69</v>
-      </c>
-      <c r="G34" t="s">
-        <v>136</v>
-      </c>
-      <c r="H34" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>61</v>
+      </c>
+      <c r="F33" t="s">
+        <v>193</v>
+      </c>
+      <c r="G33" t="s">
+        <v>194</v>
+      </c>
+      <c r="H33" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D37" t="s">
-        <v>46</v>
-      </c>
-      <c r="G37" t="s">
-        <v>77</v>
-      </c>
-      <c r="H37" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>53</v>
       </c>
       <c r="E38" t="s">
+        <v>70</v>
+      </c>
+      <c r="F38" t="s">
+        <v>69</v>
+      </c>
+      <c r="G38" t="s">
+        <v>136</v>
+      </c>
+      <c r="H38" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>46</v>
+      </c>
+      <c r="G41" t="s">
+        <v>77</v>
+      </c>
+      <c r="H41" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>53</v>
+      </c>
+      <c r="E43" t="s">
         <v>177</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F43" t="s">
         <v>179</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G43" t="s">
         <v>234</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H43" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D39" t="s">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
         <v>53</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E46" t="s">
         <v>177</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F46" t="s">
         <v>180</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G46" t="s">
         <v>235</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H46" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D40" t="s">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
         <v>53</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E48" t="s">
         <v>78</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F48" t="s">
         <v>242</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G48" t="s">
         <v>238</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H48" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D41" t="s">
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
         <v>61</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F49" t="s">
         <v>181</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G49" t="s">
         <v>183</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H49" t="s">
         <v>185</v>
       </c>
-      <c r="O41" t="s">
+      <c r="O49" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D42" t="s">
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
         <v>61</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F50" t="s">
         <v>182</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G50" t="s">
         <v>184</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H50" t="s">
         <v>186</v>
       </c>
-      <c r="O42" t="s">
+      <c r="O50" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D45" t="s">
-        <v>53</v>
-      </c>
-      <c r="E45" t="s">
-        <v>82</v>
-      </c>
-      <c r="F45" t="s">
-        <v>83</v>
-      </c>
-      <c r="G45" t="s">
-        <v>84</v>
-      </c>
-      <c r="H45" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>57</v>
-      </c>
-      <c r="C46" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D47" t="s">
-        <v>53</v>
-      </c>
-      <c r="E47" t="s">
-        <v>165</v>
-      </c>
-      <c r="F47" t="s">
-        <v>174</v>
-      </c>
-      <c r="G47" t="s">
-        <v>87</v>
-      </c>
-      <c r="H47" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D51" t="s">
-        <v>53</v>
-      </c>
-      <c r="E51" t="s">
-        <v>90</v>
-      </c>
-      <c r="F51" t="s">
-        <v>92</v>
-      </c>
-      <c r="G51" t="s">
-        <v>94</v>
-      </c>
-      <c r="H51" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>57</v>
-      </c>
-      <c r="C52" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
         <v>53</v>
       </c>
       <c r="E53" t="s">
+        <v>82</v>
+      </c>
+      <c r="F53" t="s">
+        <v>83</v>
+      </c>
+      <c r="G53" t="s">
+        <v>84</v>
+      </c>
+      <c r="H53" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>53</v>
+      </c>
+      <c r="E55" t="s">
+        <v>165</v>
+      </c>
+      <c r="F55" t="s">
+        <v>174</v>
+      </c>
+      <c r="G55" t="s">
+        <v>87</v>
+      </c>
+      <c r="H55" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>53</v>
+      </c>
+      <c r="E59" t="s">
+        <v>90</v>
+      </c>
+      <c r="F59" t="s">
+        <v>92</v>
+      </c>
+      <c r="G59" t="s">
+        <v>94</v>
+      </c>
+      <c r="H59" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>57</v>
+      </c>
+      <c r="C60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>53</v>
+      </c>
+      <c r="E61" t="s">
         <v>105</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F61" t="s">
         <v>100</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G61" t="s">
         <v>64</v>
       </c>
-      <c r="H53" t="s">
+      <c r="H61" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
         <v>57</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C63" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D56" t="s">
+    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
         <v>53</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E64" t="s">
         <v>106</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F64" t="s">
         <v>102</v>
       </c>
-      <c r="G56" t="s">
+      <c r="G64" t="s">
         <v>103</v>
       </c>
-      <c r="H56" t="s">
+      <c r="H64" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
+    <row r="65" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
+    <row r="66" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
         <v>57</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C66" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D59" t="s">
+    <row r="67" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
         <v>171</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E67" t="s">
         <v>172</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F67" t="s">
         <v>91</v>
       </c>
-      <c r="N59" t="b">
+      <c r="N67" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
+    <row r="68" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
+    <row r="69" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
+    <row r="70" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1975,17 +2069,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D111"/>
+  <dimension ref="A1:D114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20:XFD20"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.28515625" customWidth="1"/>
     <col min="4" max="4" width="43" bestFit="1" customWidth="1"/>
   </cols>
@@ -2132,218 +2226,209 @@
     </row>
     <row r="11" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>247</v>
       </c>
       <c r="B11" t="str">
-        <f>"1"</f>
-        <v>1</v>
+        <f>"D:NS,M:NS,Y:NS"</f>
+        <v>D:NS,M:NS,Y:NS</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>249</v>
       </c>
       <c r="D11" t="s">
-        <v>74</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>247</v>
       </c>
       <c r="B12" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>75</v>
+        <f>"D:1,M:1,Y:1955"</f>
+        <v>D:1,M:1,Y:1955</v>
+      </c>
+      <c r="C12" t="s">
+        <v>232</v>
+      </c>
+      <c r="D12" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" t="str">
-        <f>"3"</f>
-        <v>3</v>
-      </c>
-      <c r="C13" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" t="s">
-        <v>76</v>
-      </c>
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
     </row>
     <row r="14" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>70</v>
       </c>
       <c r="B14" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" t="str">
         <f>"9"</f>
         <v>9</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C17" t="s">
         <v>232</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D17" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15"/>
-    </row>
-    <row r="16" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B16" s="12" t="str">
-        <f>"4"</f>
-        <v>4</v>
-      </c>
-      <c r="C16" t="s">
-        <v>80</v>
-      </c>
-      <c r="D16" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B17" s="12" t="str">
-        <f>"8"</f>
-        <v>8</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>241</v>
-      </c>
-    </row>
     <row r="18" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" t="str">
-        <f>"3"</f>
-        <v>3</v>
-      </c>
-      <c r="C18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18" t="s">
-        <v>76</v>
-      </c>
+      <c r="A18" s="12"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
     </row>
     <row r="19" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>78</v>
       </c>
       <c r="B19" s="12" t="str">
+        <f>"4"</f>
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="12" t="str">
+        <f>"8"</f>
+        <v>8</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="12" t="str">
         <f>"7"</f>
         <v>7</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C22" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D22" s="12" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>177</v>
       </c>
-      <c r="B21" t="str">
+      <c r="B24" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C24" t="s">
         <v>71</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D24" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>177</v>
       </c>
-      <c r="B22" t="str">
+      <c r="B25" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C25" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D25" s="10" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>177</v>
       </c>
-      <c r="B23" t="str">
+      <c r="B26" t="str">
         <f>"9"</f>
         <v>9</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C26" t="s">
         <v>232</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D26" t="s">
         <v>233</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>82</v>
-      </c>
-      <c r="B25" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>82</v>
-      </c>
-      <c r="B26" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="D26" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>82</v>
-      </c>
-      <c r="B27" t="str">
-        <f>"3"</f>
-        <v>3</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2351,14 +2436,14 @@
         <v>82</v>
       </c>
       <c r="B28" t="str">
-        <f>"8"</f>
-        <v>8</v>
+        <f>"1"</f>
+        <v>1</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>98</v>
+        <v>71</v>
+      </c>
+      <c r="D28" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2366,78 +2451,78 @@
         <v>82</v>
       </c>
       <c r="B29" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" t="str">
+        <f>"8"</f>
+        <v>8</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" t="str">
         <f>"9"</f>
         <v>9</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C32" t="s">
         <v>232</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D32" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C30" s="16"/>
-      <c r="D30" s="14"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>90</v>
-      </c>
-      <c r="B31" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>90</v>
-      </c>
-      <c r="B32" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>75</v>
-      </c>
-    </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>90</v>
-      </c>
-      <c r="B33" t="str">
-        <f>"3"</f>
-        <v>3</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>97</v>
-      </c>
+      <c r="C33" s="16"/>
+      <c r="D33" s="14"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>90</v>
       </c>
       <c r="B34" t="str">
-        <f>"8"</f>
-        <v>8</v>
+        <f>"1"</f>
+        <v>1</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -2445,127 +2530,127 @@
         <v>90</v>
       </c>
       <c r="B35" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>90</v>
+      </c>
+      <c r="B37" t="str">
+        <f>"8"</f>
+        <v>8</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>90</v>
+      </c>
+      <c r="B38" t="str">
         <f>"9"</f>
         <v>9</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C38" t="s">
         <v>232</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D38" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="7"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="7"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>105</v>
       </c>
-      <c r="B37" t="str">
+      <c r="B40" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C40" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="D40" s="13" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>105</v>
       </c>
-      <c r="B38" t="str">
+      <c r="B41" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C41" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="D41" s="13" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>105</v>
       </c>
-      <c r="B39" t="str">
+      <c r="B42" t="str">
         <f>"9"</f>
         <v>9</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C42" t="s">
         <v>232</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D42" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>106</v>
-      </c>
-      <c r="B41" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C41" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="D41" s="13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>106</v>
-      </c>
-      <c r="B42" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="D42" s="13" t="s">
-        <v>116</v>
-      </c>
-    </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>106</v>
-      </c>
-      <c r="B43" t="str">
-        <f>"3"</f>
-        <v>3</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>117</v>
-      </c>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>106</v>
       </c>
-      <c r="B44" s="12" t="str">
-        <f>"4"</f>
-        <v>4</v>
+      <c r="B44" t="str">
+        <f>"1"</f>
+        <v>1</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -2573,30 +2658,60 @@
         <v>106</v>
       </c>
       <c r="B45" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>106</v>
+      </c>
+      <c r="B46" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>106</v>
+      </c>
+      <c r="B47" s="12" t="str">
+        <f>"4"</f>
+        <v>4</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>106</v>
+      </c>
+      <c r="B48" t="str">
         <f>"9"</f>
         <v>9</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C48" t="s">
         <v>232</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D48" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="13"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="13"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="13"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="13"/>
@@ -2649,34 +2764,38 @@
       <c r="D58" s="13"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B59" s="7"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B60" s="7"/>
+      <c r="B60" s="13"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="13"/>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B61" s="7"/>
+      <c r="B61" s="13"/>
       <c r="C61" s="13"/>
       <c r="D61" s="13"/>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" s="7"/>
-      <c r="C62" s="13"/>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" s="7"/>
-      <c r="C63" s="13"/>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" s="7"/>
-      <c r="C64" s="7"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="13"/>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" s="7"/>
-      <c r="C65" s="7"/>
+      <c r="C65" s="13"/>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" s="7"/>
+      <c r="C66" s="13"/>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" s="7"/>
@@ -2688,14 +2807,13 @@
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" s="7"/>
-      <c r="C69" s="7"/>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B71" s="15"/>
+      <c r="B71" s="7"/>
       <c r="C71" s="7"/>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
@@ -2707,7 +2825,7 @@
       <c r="C73" s="7"/>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B74" s="7"/>
+      <c r="B74" s="15"/>
       <c r="C74" s="7"/>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
@@ -2772,24 +2890,27 @@
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B90" s="7"/>
-      <c r="C90" s="15"/>
+      <c r="C90" s="7"/>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B91" s="7"/>
+      <c r="C91" s="7"/>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B92" s="7"/>
-      <c r="C92" s="15"/>
-      <c r="D92" s="15"/>
+      <c r="C92" s="7"/>
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" s="7"/>
+      <c r="C93" s="15"/>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B94" s="7"/>
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B95" s="7"/>
+      <c r="C95" s="15"/>
+      <c r="D95" s="15"/>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B96" s="7"/>
@@ -2838,6 +2959,15 @@
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B111" s="7"/>
+    </row>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B112" s="7"/>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B113" s="7"/>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B114" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -3075,11 +3205,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3304,18 +3434,18 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>193</v>
+        <v>248</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>61</v>
+        <v>246</v>
       </c>
       <c r="C17" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>193</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>61</v>
@@ -3323,37 +3453,35 @@
       <c r="C18" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="H18"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>69</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H19"/>
-      <c r="I19"/>
-    </row>
-    <row r="20" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
-        <v>179</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
+      <c r="C20" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20"/>
+      <c r="I20"/>
     </row>
     <row r="21" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>53</v>
@@ -3362,35 +3490,35 @@
         <v>0</v>
       </c>
       <c r="H21" s="20"/>
-      <c r="I21" s="12"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>242</v>
+      <c r="I21" s="20"/>
+    </row>
+    <row r="22" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
+        <v>180</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
+      <c r="C22" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" s="20"/>
+      <c r="I22" s="12"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>242</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B24" s="19" t="s">
         <v>61</v>
@@ -3398,31 +3526,31 @@
       <c r="C24" s="19" t="b">
         <v>0</v>
       </c>
+      <c r="H24" s="20"/>
       <c r="I24" s="20"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B25"/>
-      <c r="I25"/>
+    <row r="25" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" s="20"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>83</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H26"/>
+      <c r="B26"/>
       <c r="I26"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C27" s="3" t="b">
         <v>0</v>
@@ -3432,19 +3560,20 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="C28" s="3" t="b">
         <v>0</v>
       </c>
       <c r="H28"/>
+      <c r="I28"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>53</v>
@@ -3456,7 +3585,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>53</v>
@@ -3465,52 +3594,50 @@
         <v>0</v>
       </c>
       <c r="H30"/>
-      <c r="I30"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>102</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H31"/>
       <c r="I31"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C32" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="I32"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C33" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I33"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B34" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="3" t="b">
+      <c r="C34" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="I33"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>150</v>
-      </c>
-      <c r="B34" t="s">
-        <v>138</v>
-      </c>
-      <c r="C34" t="b">
-        <v>0</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>189</v>
-      </c>
+      <c r="I34"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B35" t="s">
         <v>138</v>
@@ -3521,11 +3648,10 @@
       <c r="D35" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="I35"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B36" t="s">
         <v>138</v>
@@ -3540,10 +3666,10 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B37" t="s">
-        <v>61</v>
+        <v>138</v>
       </c>
       <c r="C37" t="b">
         <v>0</v>
@@ -3555,10 +3681,10 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B38" t="s">
-        <v>138</v>
+        <v>61</v>
       </c>
       <c r="C38" t="b">
         <v>0</v>
@@ -3569,37 +3695,38 @@
       <c r="I38"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B39" s="3" t="s">
+      <c r="A39" t="s">
+        <v>153</v>
+      </c>
+      <c r="B39" t="s">
         <v>138</v>
       </c>
-      <c r="C39" s="3" t="b">
+      <c r="C39" t="b">
         <v>0</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I39"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>61</v>
+        <v>138</v>
       </c>
       <c r="C40" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>198</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="I40"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>61</v>
@@ -3607,10 +3734,13 @@
       <c r="C41" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="D41" s="3" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>61</v>
@@ -3620,10 +3750,18 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I43" s="10"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I48"/>
+      <c r="A43" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I44" s="10"/>
     </row>
     <row r="49" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I49"/>
@@ -3631,8 +3769,11 @@
     <row r="50" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I50"/>
     </row>
+    <row r="51" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I51"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I1:I50">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I1:I51">
     <sortCondition ref="I1"/>
   </sortState>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
Updates to mask question in INCL
</commit_message>
<xml_diff>
--- a/app/config/tables/MASKINCL/Forms/MASKINCL/MASKINCL.xlsx
+++ b/app/config/tables/MASKINCL/Forms/MASKINCL/MASKINCL.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2555E5-7E7F-43A5-A2A8-9C3B0522C736}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BA8D4E-596D-4E64-B431-7C8DA737936E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="269">
   <si>
     <t>setting_name</t>
   </si>
@@ -832,6 +832,15 @@
   </si>
   <si>
     <t>Família: {{data.FAM}}</t>
+  </si>
+  <si>
+    <t>No, refused</t>
+  </si>
+  <si>
+    <t>data("MASC") != "3"</t>
+  </si>
+  <si>
+    <t>Não, recusou</t>
   </si>
 </sst>
 </file>
@@ -1375,11 +1384,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
-  <dimension ref="A1:O83"/>
+  <dimension ref="A1:O85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2050,12 +2059,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="65" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="66" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
         <v>53</v>
       </c>
@@ -2072,7 +2081,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="67" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>57</v>
       </c>
@@ -2080,7 +2089,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="68" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D68" t="s">
         <v>53</v>
       </c>
@@ -2097,132 +2106,145 @@
         <v>86</v>
       </c>
     </row>
-    <row r="69" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="70" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="71" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
+        <v>57</v>
+      </c>
+      <c r="C71" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="72" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D72" t="s">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
         <v>53</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E73" t="s">
         <v>90</v>
       </c>
-      <c r="F72" t="s">
+      <c r="F73" t="s">
         <v>92</v>
       </c>
-      <c r="G72" t="s">
+      <c r="G73" t="s">
         <v>94</v>
       </c>
-      <c r="H72" t="s">
+      <c r="H73" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="73" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
         <v>57</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C74" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="74" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D74" t="s">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
         <v>53</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E75" t="s">
         <v>105</v>
       </c>
-      <c r="F74" t="s">
+      <c r="F75" t="s">
         <v>100</v>
       </c>
-      <c r="G74" t="s">
+      <c r="G75" t="s">
         <v>64</v>
       </c>
-      <c r="H74" t="s">
+      <c r="H75" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="75" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="76" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
         <v>57</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C77" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="77" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D77" t="s">
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
         <v>53</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E78" t="s">
         <v>106</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F78" t="s">
         <v>102</v>
       </c>
-      <c r="G77" t="s">
+      <c r="G78" t="s">
         <v>103</v>
       </c>
-      <c r="H77" t="s">
+      <c r="H78" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="78" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="79" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
         <v>57</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C80" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="80" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D80" t="s">
+    <row r="81" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D81" t="s">
         <v>171</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E81" t="s">
         <v>172</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F81" t="s">
         <v>91</v>
       </c>
-      <c r="N80" t="b">
+      <c r="N81" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
+    <row r="82" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
+    <row r="83" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
+    <row r="84" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="85" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2236,9 +2258,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D114"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2635,10 +2657,10 @@
         <v>3</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>72</v>
+        <v>266</v>
       </c>
       <c r="D30" t="s">
-        <v>75</v>
+        <v>268</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ready to field test
</commit_message>
<xml_diff>
--- a/app/config/tables/MASKINCL/Forms/MASKINCL/MASKINCL.xlsx
+++ b/app/config/tables/MASKINCL/Forms/MASKINCL/MASKINCL.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC5BA98-5131-4BFE-AC27-3CA33F7BD45D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2F26A5-66C6-480D-99E8-7C64FA668D70}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" tabRatio="728" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -1272,7 +1272,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1392,9 +1392,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
   <dimension ref="A1:O86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2278,9 +2278,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D114"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3300,7 +3300,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3415,8 +3415,8 @@
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>